<commit_message>
qubit on CFX finished
if for a sample both assays are measured, the script choses which measurement should be used.
</commit_message>
<xml_diff>
--- a/Qubit_on_CFX/output/results190905_QubitLAZ19-1_to_LAZ19-40.xlsx
+++ b/Qubit_on_CFX/output/results190905_QubitLAZ19-1_to_LAZ19-40.xlsx
@@ -930,7 +930,9 @@
           <t>both</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>2.464824779166207</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1024,7 +1026,9 @@
           <t>both</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>4.170888231044157</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1141,7 +1145,9 @@
           <t>both</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>4.302692002788298</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1281,7 +1287,9 @@
           <t>both</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
+      <c r="G36" t="n">
+        <v>3.871860744388574</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1306,7 +1314,9 @@
           <t>both</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
+      <c r="G37" t="n">
+        <v>5.11186148980102</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">

</xml_diff>